<commit_message>
fix calculation mistake and re-generate all result files
</commit_message>
<xml_diff>
--- a/results/confront_files/corpus_confront.xlsx
+++ b/results/confront_files/corpus_confront.xlsx
@@ -1,34 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adrac\Documents\Uni\Embeddings\metaphor_experiment\results\confront files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adrac\Documents\Uni\Embeddings\metaphor_experiment\results\confront_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C5E21A-B711-42C2-86A2-262D6FC7C6F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{C0D1EEA0-0639-456B-AAF0-6E11F2A7FC3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="250" yWindow="1140" windowWidth="18950" windowHeight="8920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300"/>
   </bookViews>
   <sheets>
     <sheet name="corpus_confront" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -41,58 +28,58 @@
     <t>mean_similarity</t>
   </si>
   <si>
-    <t>gutenberg</t>
+    <t>mean_baseline_savedBL</t>
+  </si>
+  <si>
+    <t>mean_baseline_mixedBL</t>
+  </si>
+  <si>
+    <t>mean_test_stat_savedBL</t>
+  </si>
+  <si>
+    <t>mean_test_stat_mixedBL</t>
+  </si>
+  <si>
+    <t>mean_p_value_savedBL</t>
+  </si>
+  <si>
+    <t>mean_p_value_mixedBL</t>
+  </si>
+  <si>
+    <t>amount_pos_sign_savedBL</t>
+  </si>
+  <si>
+    <t>amount_pos_sign_mixedBL</t>
+  </si>
+  <si>
+    <t>amount_pos_insign_savedBL</t>
+  </si>
+  <si>
+    <t>amount_pos_insign_mixedBL</t>
+  </si>
+  <si>
+    <t>amount_neg_sign_savedBL</t>
+  </si>
+  <si>
+    <t>amount_neg_sign_mixedBL</t>
+  </si>
+  <si>
+    <t>amount_neg_insign_savedBL</t>
+  </si>
+  <si>
+    <t>amount_neg_insign_mixedBL</t>
   </si>
   <si>
     <t>wiki</t>
   </si>
   <si>
-    <t>mean_baseline_mixedBL</t>
-  </si>
-  <si>
-    <t>mean_test_stat_mixedBL</t>
-  </si>
-  <si>
-    <t>mean_p_value_mixedBL</t>
-  </si>
-  <si>
-    <t>amount_pos_sign_mixedBL</t>
-  </si>
-  <si>
-    <t>amount_pos_insign_mixedBL</t>
-  </si>
-  <si>
-    <t>amount_neg_sign_mixedBL</t>
-  </si>
-  <si>
-    <t>amount_neg_insign_mixedBL</t>
-  </si>
-  <si>
-    <t>mean_baseline_savedBL</t>
-  </si>
-  <si>
-    <t>mean_test_stat_savedBL</t>
-  </si>
-  <si>
-    <t>mean_p_value_savedBL</t>
-  </si>
-  <si>
-    <t>amount_pos_sign_savedBL</t>
-  </si>
-  <si>
-    <t>amount_pos_insign_savedBL</t>
-  </si>
-  <si>
-    <t>amount_neg_sign_savedBL</t>
-  </si>
-  <si>
-    <t>amount_neg_insign_savedBL</t>
+    <t>gutenberg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -665,30 +652,60 @@
     <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="44">
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="124">
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color auto="1"/>
         </left>
         <right/>
-        <top/>
+        <top style="medium">
+          <color auto="1"/>
+        </top>
         <bottom/>
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -719,6 +736,1090 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="medium">
@@ -808,34 +1909,6 @@
         <right style="medium">
           <color auto="1"/>
         </right>
-        <top style="medium">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="medium">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
         <top/>
         <bottom/>
         <vertical/>
@@ -853,296 +1926,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1168,25 +1951,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:P3" totalsRowShown="0">
-  <autoFilter ref="A1:P3" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:P3" totalsRowShown="0">
+  <autoFilter ref="A1:P3"/>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="corpus"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="mean_similarity"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="mean_baseline_mixedBL" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="mean_baseline_savedBL" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="mean_test_stat_mixedBL" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="mean_test_stat_savedBL" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="mean_p_value_mixedBL" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="mean_p_value_savedBL" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="amount_pos_sign_mixedBL" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="amount_pos_sign_savedBL" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="amount_pos_insign_mixedBL" dataDxfId="5"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="amount_pos_insign_savedBL" dataDxfId="4"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="amount_neg_sign_mixedBL" dataDxfId="3"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="amount_neg_sign_savedBL" dataDxfId="2"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="amount_neg_insign_mixedBL" dataDxfId="1"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="amount_neg_insign_savedBL" dataDxfId="0"/>
+    <tableColumn id="1" name="corpus"/>
+    <tableColumn id="2" name="mean_similarity"/>
+    <tableColumn id="3" name="mean_baseline_savedBL" dataDxfId="122"/>
+    <tableColumn id="4" name="mean_baseline_mixedBL" dataDxfId="121"/>
+    <tableColumn id="5" name="mean_test_stat_savedBL" dataDxfId="120"/>
+    <tableColumn id="6" name="mean_test_stat_mixedBL" dataDxfId="119"/>
+    <tableColumn id="7" name="mean_p_value_savedBL" dataDxfId="12"/>
+    <tableColumn id="8" name="mean_p_value_mixedBL" dataDxfId="11"/>
+    <tableColumn id="9" name="amount_pos_sign_savedBL" dataDxfId="118"/>
+    <tableColumn id="10" name="amount_pos_sign_mixedBL" dataDxfId="117"/>
+    <tableColumn id="11" name="amount_pos_insign_savedBL" dataDxfId="116"/>
+    <tableColumn id="12" name="amount_pos_insign_mixedBL" dataDxfId="115"/>
+    <tableColumn id="13" name="amount_neg_sign_savedBL" dataDxfId="6"/>
+    <tableColumn id="14" name="amount_neg_sign_mixedBL" dataDxfId="5"/>
+    <tableColumn id="15" name="amount_neg_insign_savedBL" dataDxfId="0"/>
+    <tableColumn id="16" name="amount_neg_insign_mixedBL"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1481,37 +2264,37 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.08984375" customWidth="1"/>
-    <col min="3" max="3" width="17.26953125" customWidth="1"/>
-    <col min="4" max="4" width="16.54296875" customWidth="1"/>
-    <col min="5" max="5" width="15.36328125" customWidth="1"/>
-    <col min="6" max="6" width="15.81640625" customWidth="1"/>
-    <col min="7" max="7" width="15.7265625" customWidth="1"/>
-    <col min="8" max="8" width="16.08984375" customWidth="1"/>
-    <col min="9" max="9" width="26.26953125" customWidth="1"/>
-    <col min="10" max="10" width="23.1796875" customWidth="1"/>
-    <col min="11" max="11" width="11.90625" customWidth="1"/>
-    <col min="12" max="12" width="9.36328125" customWidth="1"/>
-    <col min="13" max="13" width="11.90625" customWidth="1"/>
-    <col min="14" max="14" width="10.453125" customWidth="1"/>
-    <col min="15" max="15" width="11.26953125" customWidth="1"/>
-    <col min="16" max="16" width="9.08984375" customWidth="1"/>
+    <col min="2" max="2" width="11.26953125" customWidth="1"/>
+    <col min="3" max="3" width="13.7265625" customWidth="1"/>
+    <col min="4" max="4" width="14.08984375" customWidth="1"/>
+    <col min="5" max="5" width="17.36328125" customWidth="1"/>
+    <col min="6" max="6" width="13.90625" customWidth="1"/>
+    <col min="7" max="7" width="17.6328125" customWidth="1"/>
+    <col min="8" max="8" width="15.08984375" customWidth="1"/>
+    <col min="9" max="9" width="11.54296875" customWidth="1"/>
+    <col min="10" max="10" width="10.81640625" customWidth="1"/>
+    <col min="11" max="11" width="15.1796875" customWidth="1"/>
+    <col min="12" max="12" width="13.6328125" customWidth="1"/>
+    <col min="13" max="13" width="8.36328125" customWidth="1"/>
+    <col min="14" max="14" width="10.7265625" customWidth="1"/>
+    <col min="15" max="15" width="9.08984375" customWidth="1"/>
+    <col min="16" max="16" width="14.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1522,208 +2305,208 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>12</v>
       </c>
       <c r="G1" t="s">
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="P1" t="s">
         <v>15</v>
-      </c>
-      <c r="M1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B2">
-        <v>0.20822311674133501</v>
+        <v>-0.33390010111472201</v>
       </c>
       <c r="C2" s="1">
-        <v>0.26242197904536901</v>
+        <v>-0.29536719944533701</v>
       </c>
       <c r="D2" s="2">
-        <v>0.29113396732920499</v>
+        <v>-0.29365824096796</v>
       </c>
       <c r="E2" s="1">
-        <v>-9.4856465335193398</v>
+        <v>-0.13952446599211399</v>
       </c>
       <c r="F2" s="2">
-        <v>-12.1905321711592</v>
+        <v>-0.29944271741773498</v>
       </c>
       <c r="G2" s="1">
-        <v>4.4846465898452599E-2</v>
+        <v>3.6024557846025797E-2</v>
       </c>
       <c r="H2" s="2">
-        <v>2.3332678387014302E-2</v>
+        <v>3.6087294934608299E-2</v>
       </c>
       <c r="I2" s="1">
-        <v>28</v>
+        <v>129</v>
       </c>
       <c r="J2" s="2">
+        <v>129</v>
+      </c>
+      <c r="K2" s="1">
         <v>21</v>
       </c>
-      <c r="K2" s="1">
-        <v>17</v>
-      </c>
       <c r="L2" s="2">
+        <v>18</v>
+      </c>
+      <c r="M2" s="1">
+        <v>160</v>
+      </c>
+      <c r="N2" s="2">
+        <v>161</v>
+      </c>
+      <c r="O2" s="1">
         <v>10</v>
       </c>
-      <c r="M2" s="1">
-        <v>252</v>
-      </c>
-      <c r="N2" s="2">
-        <v>281</v>
-      </c>
-      <c r="O2" s="1">
-        <v>23</v>
-      </c>
       <c r="P2" s="2">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B3">
-        <v>0.24246605238987501</v>
+        <v>-0.384192874701344</v>
       </c>
       <c r="C3" s="3">
-        <v>0.22043239865744299</v>
+        <v>-0.22557577155835401</v>
       </c>
       <c r="D3" s="4">
-        <v>0.24985526323882401</v>
+        <v>-0.225012789687558</v>
       </c>
       <c r="E3" s="3">
-        <v>2.4942338228453602</v>
+        <v>-13.103224632308301</v>
       </c>
       <c r="F3" s="4">
-        <v>-8.9051426699138098E-2</v>
+        <v>-13.278692709394999</v>
       </c>
       <c r="G3" s="3">
-        <v>0.12134516202985</v>
+        <v>1.8095179920723199E-2</v>
       </c>
       <c r="H3" s="4">
-        <v>4.4905502484559899E-2</v>
+        <v>1.8045947148830399E-2</v>
       </c>
       <c r="I3" s="3">
-        <v>145</v>
+        <v>24</v>
       </c>
       <c r="J3" s="4">
-        <v>116</v>
+        <v>23</v>
       </c>
       <c r="K3" s="3">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="L3" s="4">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="M3" s="3">
-        <v>86</v>
+        <v>281</v>
       </c>
       <c r="N3" s="4">
-        <v>168</v>
+        <v>281</v>
       </c>
       <c r="O3" s="3">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="P3" s="4">
-        <v>21</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="top10" dxfId="43" priority="50" percent="1" rank="10"/>
-    <cfRule type="top10" dxfId="42" priority="49" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="55" priority="30" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="54" priority="29" percent="1" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C3">
-    <cfRule type="top10" dxfId="41" priority="47" percent="1" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="40" priority="48" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="53" priority="27" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="52" priority="28" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D3">
-    <cfRule type="top10" dxfId="39" priority="45" percent="1" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="38" priority="46" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="51" priority="25" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="50" priority="26" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E3">
+    <cfRule type="top10" dxfId="49" priority="23" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="48" priority="24" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F3">
+    <cfRule type="top10" dxfId="47" priority="21" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="46" priority="22" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I3">
+    <cfRule type="top10" dxfId="45" priority="19" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="44" priority="20" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J3">
+    <cfRule type="top10" dxfId="43" priority="17" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="42" priority="18" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2:K3">
+    <cfRule type="top10" dxfId="41" priority="15" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="40" priority="16" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L3">
+    <cfRule type="top10" dxfId="39" priority="13" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="38" priority="14" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G3">
+    <cfRule type="top10" dxfId="37" priority="12" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="36" priority="11" percent="1" bottom="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H3">
+    <cfRule type="top10" dxfId="13" priority="10" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="14" priority="9" percent="1" bottom="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M2:M3">
+    <cfRule type="top10" dxfId="9" priority="7" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="10" priority="8" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N2:N3">
+    <cfRule type="top10" dxfId="7" priority="5" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="8" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O3">
-    <cfRule type="top10" dxfId="37" priority="23" percent="1" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="36" priority="24" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="3" priority="3" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="4" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P3">
-    <cfRule type="top10" dxfId="35" priority="21" percent="1" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="34" priority="22" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M3">
-    <cfRule type="top10" dxfId="33" priority="19" percent="1" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="32" priority="20" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N3">
-    <cfRule type="top10" dxfId="31" priority="17" percent="1" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="30" priority="18" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G3">
-    <cfRule type="top10" dxfId="29" priority="15" percent="1" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="28" priority="16" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H3">
-    <cfRule type="top10" dxfId="27" priority="13" percent="1" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="26" priority="14" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E3">
-    <cfRule type="top10" dxfId="25" priority="11" percent="1" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="24" priority="12" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F3">
-    <cfRule type="top10" dxfId="23" priority="9" percent="1" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="22" priority="10" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I3">
-    <cfRule type="top10" dxfId="21" priority="7" percent="1" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="20" priority="8" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J3">
-    <cfRule type="top10" dxfId="19" priority="5" percent="1" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="18" priority="6" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K3">
-    <cfRule type="top10" dxfId="17" priority="3" percent="1" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="16" priority="4" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L3">
-    <cfRule type="top10" dxfId="15" priority="1" percent="1" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="14" priority="2" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="1" priority="1" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="2" priority="2" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>